<commit_message>
Fixed issue when reading a scalar dataset.
</commit_message>
<xml_diff>
--- a/test/xlsx/h5readArray.xlsx
+++ b/test/xlsx/h5readArray.xlsx
@@ -8,14 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="1" r:id="rId1"/>
-    <sheet name="h5ReadArray" sheetId="5" r:id="rId2"/>
+    <sheet name="h5readArray" sheetId="6" r:id="rId2"/>
+    <sheet name="h5ReadArray1" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Home</t>
   </si>
@@ -30,6 +31,705 @@
   </si>
   <si>
     <t>Image3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+GROUP                  = INVENTORYMETADATA
+  GROUPTYPE            = MASTERGROUP
+  GROUP                  = ECSDATAGRANULE
+    OBJECT                 = REPROCESSINGPLANNED
+      NUM_VAL              = 1
+      VALUE                = "further update anticipated using enhanced PGE"
+    END_OBJECT             = REPROCESSINGPLANNED
+    OBJECT                 = REPROCESSINGACTUAL
+      NUM_VAL              = 1
+      VALUE                = "processed once"
+    END_OBJECT             = REPROCESSINGACTUAL
+    OBJECT                 = LOCALGRANULEID
+      NUM_VAL              = 1
+      VALUE                = "../../HIRDLS2_v2.04.09-c3_2008d001.he5"
+    END_OBJECT             = LOCALGRANULEID
+    OBJECT                 = DAYNIGHTFLAG
+      NUM_VAL              = 1
+      VALUE                = "Both"
+    END_OBJECT             = DAYNIGHTFLAG
+    OBJECT                 = PRODUCTIONDATETIME
+      NUM_VAL              = 1
+      VALUE                = "2008-01-23T06:06:07.000Z"
+    END_OBJECT             = PRODUCTIONDATETIME
+    OBJECT                 = LOCALVERSIONID
+      NUM_VAL              = 1
+      VALUE                = "2.04.09"
+    END_OBJECT             = LOCALVERSIONID
+  END_GROUP              = ECSDATAGRANULE
+  GROUP                  = MEASUREDPARAMETER
+    OBJECT                 = MEASUREDPARAMETERCONTAINER
+      CLASS                = "1"
+      OBJECT                 = PARAMETERNAME
+        NUM_VAL              = 1
+        CLASS                = "1"
+        VALUE                = "Atmospheric Pressure"
+      END_OBJECT             = PARAMETERNAME
+      GROUP                  = QAFLAGS
+        CLASS                = "1"
+        OBJECT                 = AUTOMATICQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "1"
+          VALUE                = "Suspect"
+        END_OBJECT             = AUTOMATICQUALITYFLAG
+        OBJECT                 = AUTOMATICQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "1"
+          VALUE                = "Process Terminated Normally - Check Science Quality Flag for Science Team quality assessment"
+        END_OBJECT             = AUTOMATICQUALITYFLAGEXPLANATION
+        OBJECT                 = OPERATIONALQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "1"
+          VALUE                = "Not Investigated"
+        END_OBJECT             = OPERATIONALQUALITYFLAG
+        OBJECT                 = OPERATIONALQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "1"
+          VALUE                = "Q/A process has not yet been run"
+        END_OBJECT             = OPERATIONALQUALITYFLAGEXPLANATION
+        OBJECT                 = SCIENCEQUALITYFLAG
+          NUM_VAL              = 1
+          VALUE                = "Not Investigated"
+          CLASS                = "1"
+        END_OBJECT             = SCIENCEQUALITYFLAG
+      END_GROUP              = QAFLAGS
+      GROUP                  = QASTATS
+        CLASS                = "1"
+        OBJECT                 = QAPERCENTMISSINGDATA
+          NUM_VAL              = 1
+          CLASS                = "1"
+          VALUE                = 0
+        END_OBJECT             = QAPERCENTMISSINGDATA
+        OBJECT                 = QAPERCENTOUTOFBOUNDSDATA
+          NUM_VAL              = 1
+          CLASS                = "1"
+          VALUE                = 0
+        END_OBJECT             = QAPERCENTOUTOFBOUNDSDATA
+      END_GROUP              = QASTATS
+    END_OBJECT             = MEASUREDPARAMETERCONTAINER
+    OBJECT                 = MEASUREDPARAMETERCONTAINER
+      CLASS                = "2"
+      OBJECT                 = PARAMETERNAME
+        NUM_VAL              = 1
+        CLASS                = "2"
+        VALUE                = "Temperature Profile"
+      END_OBJECT             = PARAMETERNAME
+      GROUP                  = QAFLAGS
+        CLASS                = "2"
+        OBJECT                 = AUTOMATICQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "2"
+          VALUE                = "Suspect"
+        END_OBJECT             = AUTOMATICQUALITYFLAG
+        OBJECT                 = AUTOMATICQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "2"
+          VALUE                = "Process Terminated Normally - Check Science Quality Flag for Science Team quality assessment"
+        END_OBJECT             = AUTOMATICQUALITYFLAGEXPLANATION
+        OBJECT                 = OPERATIONALQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "2"
+          VALUE                = "Not Investigated"
+        END_OBJECT             = OPERATIONALQUALITYFLAG
+        OBJECT                 = OPERATIONALQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "2"
+          VALUE                = "Q/A process has not yet been run"
+        END_OBJECT             = OPERATIONALQUALITYFLAGEXPLANATION
+        OBJECT                 = SCIENCEQUALITYFLAG
+          NUM_VAL              = 1
+          VALUE                = "Not Investigated"
+          CLASS                = "2"
+        END_OBJECT             = SCIENCEQUALITYFLAG
+      END_GROUP              = QAFLAGS
+      GROUP                  = QASTATS
+        CLASS                = "2"
+        OBJECT                 = QAPERCENTMISSINGDATA
+          NUM_VAL              = 1
+          CLASS                = "2"
+          VALUE                = 38
+        END_OBJECT             = QAPERCENTMISSINGDATA
+        OBJECT                 = QAPERCENTOUTOFBOUNDSDATA
+          NUM_VAL              = 1
+          CLASS                = "2"
+          VALUE                = 0
+        END_OBJECT             = QAPERCENTOUTOFBOUNDSDATA
+      END_GROUP              = QASTATS
+    END_OBJECT             = MEASUREDPARAMETERCONTAINER
+    OBJECT                 = MEASUREDPARAMETERCONTAINER
+      CLASS                = "3"
+      OBJECT                 = PARAMETERNAME
+        NUM_VAL              = 1
+        CLASS                = "3"
+        VALUE                = "Water Vapor"
+      END_OBJECT             = PARAMETERNAME
+      GROUP                  = QAFLAGS
+        CLASS                = "3"
+        OBJECT                 = AUTOMATICQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "3"
+          VALUE                = "Suspect"
+        END_OBJECT             = AUTOMATICQUALITYFLAG
+        OBJECT                 = AUTOMATICQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "3"
+          VALUE                = "Process Terminated Normally - Check Science Quality Flag for Science Team quality assessment"
+        END_OBJECT             = AUTOMATICQUALITYFLAGEXPLANATION
+        OBJECT                 = OPERATIONALQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "3"
+          VALUE                = "Not Investigated"
+        END_OBJECT             = OPERATIONALQUALITYFLAG
+        OBJECT                 = OPERATIONALQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "3"
+          VALUE                = "Q/A process has not yet been run"
+        END_OBJECT             = OPERATIONALQUALITYFLAGEXPLANATION
+        OBJECT                 = SCIENCEQUALITYFLAG
+          NUM_VAL              = 1
+          VALUE                = "Not Investigated"
+          CLASS                = "3"
+        END_OBJECT             = SCIENCEQUALITYFLAG
+      END_GROUP              = QAFLAGS
+      GROUP                  = QASTATS
+        CLASS                = "3"
+        OBJECT                 = QAPERCENTMISSINGDATA
+          NUM_VAL              = 1
+          CLASS                = "3"
+          VALUE                = 48
+        END_OBJECT             = QAPERCENTMISSINGDATA
+        OBJECT                 = QAPERCENTOUTOFBOUNDSDATA
+          NUM_VAL              = 1
+          CLASS                = "3"
+          VALUE                = 0
+        END_OBJECT             = QAPERCENTOUTOFBOUNDSDATA
+      END_GROUP              = QASTATS
+    END_OBJECT             = MEASUREDPARAMETERCONTAINER
+    OBJECT                 = MEASUREDPARAMETERCONTAINER
+      CLASS                = "4"
+      OBJECT                 = PARAMETERNAME
+        NUM_VAL              = 1
+        CLASS                = "4"
+        VALUE                = "Chlorofluorocarbon-11"
+      END_OBJECT             = PARAMETERNAME
+      GROUP                  = QAFLAGS
+        CLASS                = "4"
+        OBJECT                 = AUTOMATICQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "4"
+          VALUE                = "Suspect"
+        END_OBJECT             = AUTOMATICQUALITYFLAG
+        OBJECT                 = AUTOMATICQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "4"
+          VALUE                = "Process Terminated Normally - Check Science Quality Flag for Science Team quality assessment"
+        END_OBJECT             = AUTOMATICQUALITYFLAGEXPLANATION
+        OBJECT                 = OPERATIONALQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "4"
+          VALUE                = "Not Investigated"
+        END_OBJECT             = OPERATIONALQUALITYFLAG
+        OBJECT                 = OPERATIONALQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "4"
+          VALUE                = "Q/A process has not yet been run"
+        END_OBJECT             = OPERATIONALQUALITYFLAGEXPLANATION
+        OBJECT                 = SCIENCEQUALITYFLAG
+          NUM_VAL              = 1
+          VALUE                = "Not Investigated"
+          CLASS                = "4"
+        END_OBJECT             = SCIENCEQUALITYFLAG
+      END_GROUP              = QAFLAGS
+      GROUP                  = QASTATS
+        CLASS                = "4"
+        OBJECT                 = QAPERCENTMISSINGDATA
+          NUM_VAL              = 1
+          CLASS                = "4"
+          VALUE                = 59
+        END_OBJECT             = QAPERCENTMISSINGDATA
+        OBJECT                 = QAPERCENTOUTOFBOUNDSDATA
+          NUM_VAL              = 1
+          CLASS                = "4"
+          VALUE                = 0
+        END_OBJECT             = QAPERCENTOUTOFBOUNDSDATA
+      END_GROUP              = QASTATS
+    END_OBJECT             = MEASUREDPARAMETERCONTAINER
+    OBJECT                 = MEASUREDPARAMETERCONTAINER
+      CLASS                = "5"
+      OBJECT                 = PARAMETERNAME
+        NUM_VAL              = 1
+        CLASS                = "5"
+        VALUE                = "Chlorofluorocarbon-12"
+      END_OBJECT             = PARAMETERNAME
+      GROUP                  = QAFLAGS
+        CLASS                = "5"
+        OBJECT                 = AUTOMATICQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "5"
+          VALUE                = "Suspect"
+        END_OBJECT             = AUTOMATICQUALITYFLAG
+        OBJECT                 = AUTOMATICQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "5"
+          VALUE                = "Process Terminated Normally - Check Science Quality Flag for Science Team quality assessment"
+        END_OBJECT             = AUTOMATICQUALITYFLAGEXPLANATION
+        OBJECT                 = OPERATIONALQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "5"
+          VALUE                = "Not Investigated"
+        END_OBJECT             = OPERATIONALQUALITYFLAG
+        OBJECT                 = OPERATIONALQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "5"
+          VALUE                = "Q/A process has not yet been run"
+        END_OBJECT             = OPERATIONALQUALITYFLAGEXPLANATION
+        OBJECT                 = SCIENCEQUALITYFLAG
+          NUM_VAL              = 1
+          VALUE                = "Not Investigated"
+          CLASS                = "5"
+        END_OBJECT             = SCIENCEQUALITYFLAG
+      END_GROUP              = QAFLAGS
+      GROUP                  = QASTATS
+        CLASS                = "5"
+        OBJECT                 = QAPERCENTMISSINGDATA
+          NUM_VAL              = 1
+          CLASS                = "5"
+          VALUE                = 59
+        END_OBJECT             = QAPERCENTMISSINGDATA
+        OBJECT                 = QAPERCENTOUTOFBOUNDSDATA
+          NUM_VAL              = 1
+          CLASS                = "5"
+          VALUE                = 0
+        END_OBJECT             = QAPERCENTOUTOFBOUNDSDATA
+      END_GROUP              = QASTATS
+    END_OBJECT             = MEASUREDPARAMETERCONTAINER
+    OBJECT                 = MEASUREDPARAMETERCONTAINER
+      CLASS                = "6"
+      OBJECT                 = PARAMETERNAME
+        NUM_VAL              = 1
+        CLASS                = "6"
+        VALUE                = "Ozone"
+      END_OBJECT             = PARAMETERNAME
+      GROUP                  = QAFLAGS
+        CLASS                = "6"
+        OBJECT                 = AUTOMATICQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "6"
+          VALUE                = "Suspect"
+        END_OBJECT             = AUTOMATICQUALITYFLAG
+        OBJECT                 = AUTOMATICQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "6"
+          VALUE                = "Process Terminated Normally - Check Science Quality Flag for Science Team quality assessment"
+        END_OBJECT             = AUTOMATICQUALITYFLAGEXPLANATION
+        OBJECT                 = OPERATIONALQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "6"
+          VALUE                = "Not Investigated"
+        END_OBJECT             = OPERATIONALQUALITYFLAG
+        OBJECT                 = OPERATIONALQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "6"
+          VALUE                = "Q/A process has not yet been run"
+        END_OBJECT             = OPERATIONALQUALITYFLAGEXPLANATION
+        OBJECT                 = SCIENCEQUALITYFLAG
+          NUM_VAL              = 1
+          VALUE                = "Not Investigated"
+          CLASS                = "6"
+        END_OBJECT             = SCIENCEQUALITYFLAG
+      END_GROUP              = QAFLAGS
+      GROUP                  = QASTATS
+        CLASS                = "6"
+        OBJECT                 = QAPERCENTMISSINGDATA
+          NUM_VAL              = 1
+          CLASS                = "6"
+          VALUE                = 38
+        END_OBJECT             = QAPERCENTMISSINGDATA
+        OBJECT                 = QAPERCENTOUTOFBOUNDSDATA
+          NUM_VAL              = 1
+          CLASS                = "6"
+          VALUE                = 0
+        END_OBJECT             = QAPERCENTOUTOFBOUNDSDATA
+      END_GROUP              = QASTATS
+    END_OBJECT             = MEASUREDPARAMETERCONTAINER
+    OBJECT                 = MEASUREDPARAMETERCONTAINER
+      CLASS                = "7"
+      OBJECT                 = PARAMETERNAME
+        NUM_VAL              = 1
+        CLASS                = "7"
+        VALUE                = "Nitric Acid"
+      END_OBJECT             = PARAMETERNAME
+      GROUP                  = QAFLAGS
+        CLASS                = "7"
+        OBJECT                 = AUTOMATICQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "7"
+          VALUE                = "Suspect"
+        END_OBJECT             = AUTOMATICQUALITYFLAG
+        OBJECT                 = AUTOMATICQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "7"
+          VALUE                = "Process Terminated Normally - Check Science Quality Flag for Science Team quality assessment"
+        END_OBJECT             = AUTOMATICQUALITYFLAGEXPLANATION
+        OBJECT                 = OPERATIONALQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "7"
+          VALUE                = "Not Investigated"
+        END_OBJECT             = OPERATIONALQUALITYFLAG
+        OBJECT                 = OPERATIONALQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "7"
+          VALUE                = "Q/A process has not yet been run"
+        END_OBJECT             = OPERATIONALQUALITYFLAGEXPLANATION
+        OBJECT                 = SCIENCEQUALITYFLAG
+          NUM_VAL              = 1
+          VALUE                = "Not Investigated"
+          CLASS                = "7"
+        END_OBJECT             = SCIENCEQUALITYFLAG
+      END_GROUP              = QAFLAGS
+      GROUP                  = QASTATS
+        CLASS                = "7"
+        OBJECT                 = QAPERCENTMISSINGDATA
+          NUM_VAL              = 1
+          CLASS                = "7"
+          VALUE                = 59
+        END_OBJECT             = QAPERCENTMISSINGDATA
+        OBJECT                 = QAPERCENTOUTOFBOUNDSDATA
+          NUM_VAL              = 1
+          CLASS                = "7"
+          VALUE                = 1
+        END_OBJECT             = QAPERCENTOUTOFBOUNDSDATA
+      END_GROUP              = QASTATS
+    END_OBJECT             = MEASUREDPARAMETERCONTAINER
+    OBJECT                 = MEASUREDPARAMETERCONTAINER
+      CLASS                = "8"
+      OBJECT                 = PARAMETERNAME
+        NUM_VAL              = 1
+        CLASS                = "8"
+        VALUE                = "Dinitrogen Pentoxide"
+      END_OBJECT             = PARAMETERNAME
+      GROUP                  = QAFLAGS
+        CLASS                = "8"
+        OBJECT                 = AUTOMATICQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "8"
+          VALUE                = "Suspect"
+        END_OBJECT             = AUTOMATICQUALITYFLAG
+        OBJECT                 = AUTOMATICQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "8"
+          VALUE                = "Process Terminated Normally - Check Science Quality Flag for Science Team quality assessment"
+        END_OBJECT             = AUTOMATICQUALITYFLAGEXPLANATION
+        OBJECT                 = OPERATIONALQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "8"
+          VALUE                = "Not Investigated"
+        END_OBJECT             = OPERATIONALQUALITYFLAG
+        OBJECT                 = OPERATIONALQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "8"
+          VALUE                = "Q/A process has not yet been run"
+        END_OBJECT             = OPERATIONALQUALITYFLAGEXPLANATION
+        OBJECT                 = SCIENCEQUALITYFLAG
+          NUM_VAL              = 1
+          VALUE                = "Not Investigated"
+          CLASS                = "8"
+        END_OBJECT             = SCIENCEQUALITYFLAG
+      END_GROUP              = QAFLAGS
+      GROUP                  = QASTATS
+        CLASS                = "8"
+        OBJECT                 = QAPERCENTMISSINGDATA
+          NUM_VAL              = 1
+          CLASS                = "8"
+          VALUE                = 60
+        END_OBJECT             = QAPERCENTMISSINGDATA
+        OBJECT                 = QAPERCENTOUTOFBOUNDSDATA
+          NUM_VAL              = 1
+          CLASS                = "8"
+          VALUE                = 3
+        END_OBJECT             = QAPERCENTOUTOFBOUNDSDATA
+      END_GROUP              = QASTATS
+    END_OBJECT             = MEASUREDPARAMETERCONTAINER
+    OBJECT                 = MEASUREDPARAMETERCONTAINER
+      CLASS                = "9"
+      OBJECT                 = PARAMETERNAME
+        NUM_VAL              = 1
+        CLASS                = "9"
+        VALUE                = "Nitrous Oxide"
+      END_OBJECT             = PARAMETERNAME
+      GROUP                  = QAFLAGS
+        CLASS                = "9"
+        OBJECT                 = AUTOMATICQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "9"
+          VALUE                = "Suspect"
+        END_OBJECT             = AUTOMATICQUALITYFLAG
+        OBJECT                 = AUTOMATICQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "9"
+          VALUE                = "Process Terminated Normally - Check Science Quality Flag for Science Team quality assessment"
+        END_OBJECT             = AUTOMATICQUALITYFLAGEXPLANATION
+        OBJECT                 = OPERATIONALQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "9"
+          VALUE                = "Not Investigated"
+        END_OBJECT             = OPERATIONALQUALITYFLAG
+        OBJECT                 = OPERATIONALQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "9"
+          VALUE                = "Q/A process has not yet been run"
+        END_OBJECT             = OPERATIONALQUALITYFLAGEXPLANATION
+        OBJECT                 = SCIENCEQUALITYFLAG
+          NUM_VAL              = 1
+          VALUE                = "Not Investigated"
+          CLASS                = "9"
+        END_OBJECT             = SCIENCEQUALITYFLAG
+      END_GROUP              = QAFLAGS
+      GROUP                  = QASTATS
+        CLASS                = "9"
+        OBJECT                 = QAPERCENTMISSINGDATA
+          NUM_VAL              = 1
+          CLASS                = "9"
+          VALUE                = 60
+        END_OBJECT             = QAPERCENTMISSINGDATA
+        OBJECT                 = QAPERCENTOUTOFBOUNDSDATA
+          NUM_VAL              = 1
+          CLASS                = "9"
+          VALUE                = 0
+        END_OBJECT             = QAPERCENTOUTOFBOUNDSDATA
+      END_GROUP              = QASTATS
+    END_OBJECT             = MEASUREDPARAMETERCONTAINER
+    OBJECT                 = MEASUREDPARAMETERCONTAINER
+      CLASS                = "10"
+      OBJECT                 = PARAMETERNAME
+        NUM_VAL              = 1
+        CLASS                = "10"
+        VALUE                = "Chlorine Nitrate"
+      END_OBJECT             = PARAMETERNAME
+      GROUP                  = QAFLAGS
+        CLASS                = "10"
+        OBJECT                 = AUTOMATICQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "10"
+          VALUE                = "Suspect"
+        END_OBJECT             = AUTOMATICQUALITYFLAG
+        OBJECT                 = AUTOMATICQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "10"
+          VALUE                = "Process Terminated Normally - Check Science Quality Flag for Science Team quality assessment"
+        END_OBJECT             = AUTOMATICQUALITYFLAGEXPLANATION
+        OBJECT                 = OPERATIONALQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "10"
+          VALUE                = "Not Investigated"
+        END_OBJECT             = OPERATIONALQUALITYFLAG
+        OBJECT                 = OPERATIONALQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "10"
+          VALUE                = "Q/A process has not yet been run"
+        END_OBJECT             = OPERATIONALQUALITYFLAGEXPLANATION
+        OBJECT                 = SCIENCEQUALITYFLAG
+          NUM_VAL              = 1
+          VALUE                = "Not Investigated"
+          CLASS                = "10"
+        END_OBJECT             = SCIENCEQUALITYFLAG
+      END_GROUP              = QAFLAGS
+      GROUP                  = QASTATS
+        CLASS                = "10"
+        OBJECT                 = QAPERCENTMISSINGDATA
+          NUM_VAL              = 1
+          CLASS                = "10"
+          VALUE                = 60
+        END_OBJECT             = QAPERCENTMISSINGDATA
+        OBJECT                 = QAPERCENTOUTOFBOUNDSDATA
+          NUM_VAL              = 1
+          CLASS                = "10"
+          VALUE                = 0
+        END_OBJECT             = QAPERCENTOUTOFBOUNDSDATA
+      END_GROUP              = QASTATS
+    END_OBJECT             = MEASUREDPARAMETERCONTAINER
+    OBJECT                 = MEASUREDPARAMETERCONTAINER
+      CLASS                = "11"
+      OBJECT                 = PARAMETERNAME
+        NUM_VAL              = 1
+        CLASS                = "11"
+        VALUE                = "Nitrogen Dioxide"
+      END_OBJECT             = PARAMETERNAME
+      GROUP                  = QAFLAGS
+        CLASS                = "11"
+        OBJECT                 = AUTOMATICQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "11"
+          VALUE                = "Suspect"
+        END_OBJECT             = AUTOMATICQUALITYFLAG
+        OBJECT                 = AUTOMATICQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "11"
+          VALUE                = "Process Terminated Normally - Check Science Quality Flag for Science Team quality assessment"
+        END_OBJECT             = AUTOMATICQUALITYFLAGEXPLANATION
+        OBJECT                 = OPERATIONALQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "11"
+          VALUE                = "Not Investigated"
+        END_OBJECT             = OPERATIONALQUALITYFLAG
+        OBJECT                 = OPERATIONALQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "11"
+          VALUE                = "Q/A process has not yet been run"
+        END_OBJECT             = OPERATIONALQUALITYFLAGEXPLANATION
+        OBJECT                 = SCIENCEQUALITYFLAG
+          NUM_VAL              = 1
+          VALUE                = "Not Investigated"
+          CLASS                = "11"
+        END_OBJECT             = SCIENCEQUALITYFLAG
+      END_GROUP              = QAFLAGS
+      GROUP                  = QASTATS
+        CLASS                = "11"
+        OBJECT                 = QAPERCENTMISSINGDATA
+          NUM_VAL              = 1
+          CLASS                = "11"
+          VALUE                = 51
+        END_OBJECT             = QAPERCENTMISSINGDATA
+        OBJECT                 = QAPERCENTOUTOFBOUNDSDATA
+          NUM_VAL              = 1
+          CLASS                = "11"
+          VALUE                = 1
+        END_OBJECT             = QAPERCENTOUTOFBOUNDSDATA
+      END_GROUP              = QASTATS
+    END_OBJECT             = MEASUREDPARAMETERCONTAINER
+    OBJECT                 = MEASUREDPARAMETERCONTAINER
+      CLASS                = "12"
+      OBJECT                 = PARAMETERNAME
+        NUM_VAL              = 1
+        CLASS                = "12"
+        VALUE                = "Methane"
+      END_OBJECT             = PARAMETERNAME
+      GROUP                  = QAFLAGS
+        CLASS                = "12"
+        OBJECT                 = AUTOMATICQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "12"
+          VALUE                = "Suspect"
+        END_OBJECT             = AUTOMATICQUALITYFLAG
+        OBJECT                 = AUTOMATICQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "12"
+          VALUE                = "Process Terminated Normally - Check Science Quality Flag for Science Team quality assessment"
+        END_OBJECT             = AUTOMATICQUALITYFLAGEXPLANATION
+        OBJECT                 = OPERATIONALQUALITYFLAG
+          NUM_VAL              = 1
+          CLASS                = "12"
+          VALUE                = "Not Investigated"
+        END_OBJECT             = OPERATIONALQUALITYFLAG
+        OBJECT                 = OPERATIONALQUALITYFLAGEXPLANATION
+          NUM_VAL              = 1
+          CLASS                = "12"
+          VALUE                = "Q/A process has not yet been run"
+        END_OBJECT             = OPERATIONALQUALITYFLAGEXPLANATION
+        OBJECT                 = SCIENCEQUALITYFLAG
+          NUM_VAL              = 1
+          VALUE                = "Not Investigated"
+          CLASS                = "12"
+        END_OBJECT             = SCIENCEQUALITYFLAG
+      END_GROUP              = QAFLAGS
+      GROUP                  = QASTATS
+        CLASS                = "12"
+        OBJECT                 = QAPERCENTMISSINGDATA
+          NUM_VAL              = 1
+          CLASS                = "12"
+          VALUE                = 60
+        END_OBJECT             = QAPERCENTMISSINGDATA
+        OBJECT                 = QAPERCENTOUTOFBOUNDSDATA
+          NUM_VAL              = 1
+          CLASS                = "12"
+          VALUE                = 1
+        END_OBJECT             = QAPERCENTOUTOFBOUNDSDATA
+      END_GROUP              = QASTATS
+    END_OBJECT             = MEASUREDPARAMETERCONTAINER
+  END_GROUP              = MEASUREDPARAMETER
+  GROUP                  = COLLECTIONDESCRIPTIONCLASS
+    OBJECT                 = SHORTNAME
+      NUM_VAL              = 1
+      VALUE                = "HIRDLS2"
+    END_OBJECT             = SHORTNAME
+    OBJECT                 = VERSIONID
+      NUM_VAL              = 1
+      VALUE                = 3
+    END_OBJECT             = VERSIONID
+  END_GROUP              = COLLECTIONDESCRIPTIONCLASS
+  GROUP                  = INPUTGRANULE
+    OBJECT                 = INPUTPOINTER
+      NUM_VAL              = 1
+      VALUE                = "See Production History File for this information"
+    END_OBJECT             = INPUTPOINTER
+  END_GROUP              = INPUTGRANULE
+  GROUP                  = SPATIALDOMAINCONTAINER
+    GROUP                  = GRANULELOCALITY
+      OBJECT                 = LOCALITYVALUE
+        NUM_VAL              = 1
+        VALUE                = "Global"
+      END_OBJECT             = LOCALITYVALUE
+    END_GROUP              = GRANULELOCALITY
+    GROUP                  = VERTICALSPATIALDOMAIN
+      OBJECT                 = VERTICALSPATIALDOMAINCONTAINER
+        CLASS                = "1"
+        OBJECT                 = VERTICALSPATIALDOMAINTYPE
+          CLASS                = "1"
+          NUM_VAL              = 1
+          VALUE                = "Atmosphere Layer"
+        END_OBJECT             = VERTICALSPATIALDOMAINTYPE
+        OBJECT                 = VERTICALSPATIALDOMAINVALUE
+          CLASS                = "1"
+          NUM_VAL              = 1
+          VALUE                = "Atmosphere Profile"
+        END_OBJECT             = VERTICALSPATIALDOMAINVALUE
+      END_OBJECT             = VERTICALSPATIALDOMAINCONTAINER
+    END_GROUP              = VERTICALSPATIALDOMAIN
+    GROUP                  = HORIZONTALSPATIALDOMAINCONTAINER
+      GROUP                  = BOUNDINGRECTANGLE
+        OBJECT                 = WESTBOUNDINGCOORDINATE
+          NUM_VAL              = 1
+          VALUE                = -180.0
+        END_OBJECT             = WESTBOUNDINGCOORDINATE
+        OBJECT                 = NORTHBOUNDINGCOORDINATE
+          NUM_VAL              = 1
+          VALUE                = 90.0
+        END_OBJECT             = NORTHBOUNDINGCOORDINATE
+        OBJECT                 = EASTBOUNDINGCOORDINATE
+          NUM_VAL              = 1
+          VALUE                = 180.0
+        END_OBJECT             = EASTBOUNDINGCOORDINATE
+        OBJECT                 = SOUTHBOUNDINGCOORDINATE
+          NUM_VAL              = 1
+          VALUE                = -90.0
+        END_OBJECT             = SOUTHBOUNDINGCOORDINATE
+      END_GROUP              = BOUNDINGRECTANGLE
+    END_GROUP              = HORIZONTALSPATIALDOMAINCONTAINER
+  END_GROUP              = SPATIALDOMAINCONTAINER
+  GROUP                  = RANGEDATETIME
+    OBJECT                 = RANGEBEGINNINGDATE
+      NUM_VAL              = 1
+      VALUE                = "2008-01-01"
+    END_OBJECT             = RANGEBEGINNINGDATE
+    OBJECT                 = RANGEBEGINNINGTIME
+      NUM_VAL              = 1
+      VALUE                = "00:00:09.45"
+    END_OBJECT             = RANGEBEGINNINGTIME
+    OBJECT                 = RANGEENDINGDATE
+      NUM_VAL              = 1
+      VALUE                = "2008-01-01"
+    END_OBJECT             = RANGEENDINGDATE
+    OBJECT                 = RANGEENDINGTIME
+      NUM_VAL              = 1
+      VALUE                = "23:59:48.11"
+    END_OBJECT             = RANGEENDINGTIME
+  END_GROUP              = RANGEDATETIME
+  GROUP               </t>
   </si>
 </sst>
 </file>
@@ -73,10 +773,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,9 +1149,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="77.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="str">
+        <f ca="1">_xll.h5readArray(Globals!B2, "/HDFEOS INFORMATION/coremetadata.0")</f>
+        <v>1 x 1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z557"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
h5show[List,Tree] echo the file name.
Fixed "infinite cycle" in example workbooks.
</commit_message>
<xml_diff>
--- a/test/xlsx/h5readArray.xlsx
+++ b/test/xlsx/h5readArray.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Home</t>
   </si>
@@ -731,12 +731,15 @@
   END_GROUP              = RANGEDATETIME
   GROUP               </t>
   </si>
+  <si>
+    <t>C:\Users\Gerd\git\PyHexad\</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -752,13 +755,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -773,13 +789,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1086,7 +1103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1100,9 +1117,8 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="str">
-        <f ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"),1)-1)</f>
-        <v>C:\Users\Gerd\git\PyHexad\test\xlsx\</v>
+      <c r="B1" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1110,8 +1126,8 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <f ca="1">CONCATENATE($B1,"..\..\testfiles\hdfeos5.h5")</f>
-        <v>C:\Users\Gerd\git\PyHexad\test\xlsx\..\..\testfiles\hdfeos5.h5</v>
+        <f>CONCATENATE($B1,"testfiles\hdfeos5.h5")</f>
+        <v>C:\Users\Gerd\git\PyHexad\testfiles\hdfeos5.h5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1119,8 +1135,8 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <f ca="1">CONCATENATE($B1,"..\..\testfiles\tall_with_udlink.h5")</f>
-        <v>C:\Users\Gerd\git\PyHexad\test\xlsx\..\..\testfiles\tall_with_udlink.h5</v>
+        <f>CONCATENATE($B1,"testfiles\tall_with_udlink.h5")</f>
+        <v>C:\Users\Gerd\git\PyHexad\testfiles\tall_with_udlink.h5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1128,8 +1144,8 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <f ca="1">CONCATENATE($B1,"..\..\testfiles\group100.h5")</f>
-        <v>C:\Users\Gerd\git\PyHexad\test\xlsx\..\..\testfiles\group100.h5</v>
+        <f>CONCATENATE($B1,"testfiles\group100.h5")</f>
+        <v>C:\Users\Gerd\git\PyHexad\testfiles\group100.h5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1137,8 +1153,8 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <f ca="1">CONCATENATE($B1,"..\..\testfiles\ex_image3.h5")</f>
-        <v>C:\Users\Gerd\git\PyHexad\test\xlsx\..\..\testfiles\ex_image3.h5</v>
+        <f>CONCATENATE($B1,"testfiles\ex_image3.h5")</f>
+        <v>C:\Users\Gerd\git\PyHexad\testfiles\ex_image3.h5</v>
       </c>
     </row>
   </sheetData>
@@ -1151,7 +1167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1160,7 +1176,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
-        <f ca="1">_xll.h5readArray(Globals!B2, "/HDFEOS INFORMATION/coremetadata.0")</f>
+        <f>_xll.h5readArray(Globals!B2, "/HDFEOS INFORMATION/coremetadata.0")</f>
         <v>1 x 1</v>
       </c>
     </row>
@@ -1190,11 +1206,11 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
-        <f ca="1">_xll.h5readArray(Globals!B2,"/HDFEOS/SWATHS/HIRDLS/Geolocation Fields/Latitude",{8},{5500},{20})</f>
+        <f>_xll.h5readArray(Globals!B2,"/HDFEOS/SWATHS/HIRDLS/Geolocation Fields/Latitude",{8},{5500},{20})</f>
         <v>275 x 1</v>
       </c>
       <c r="C1" t="str">
-        <f ca="1">_xll.h5readArray(Globals!B2,"/HDFEOS/SWATHS/HIRDLS/Data Fields/O3", {8,10}, {5500,80}, {20,3})</f>
+        <f>_xll.h5readArray(Globals!B2,"/HDFEOS/SWATHS/HIRDLS/Data Fields/O3", {8,10}, {5500,80}, {20,3})</f>
         <v>275 x 24</v>
       </c>
     </row>

</xml_diff>